<commit_message>
Pruebas con visualizador de matrices
</commit_message>
<xml_diff>
--- a/Jupyter Notebook/Cálculos de Matriz.xlsx
+++ b/Jupyter Notebook/Cálculos de Matriz.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulise\Documents\UV\9° semestre\GTS\Material de Apoyo\Jupyter Notebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulise\Documents\UV\9° semestre\GTS\Jupyter Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5982D421-EEA0-4878-8FE0-52F60FB2FF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A4F04A-ADD0-4846-B234-F11AADBF23F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AA86D61-9D76-B74F-AA0D-E6B0A4E37F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2AA86D61-9D76-B74F-AA0D-E6B0A4E37F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Total de Escenarios Estrategias" sheetId="3" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -457,13 +458,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -906,26 +907,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C68D51D-B8CB-4062-B34D-A024901C524E}">
   <dimension ref="B1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="2:19">
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="2:19">
       <c r="B2" s="5"/>
@@ -1428,19 +1429,19 @@
       </c>
     </row>
     <row r="18" spans="3:21">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
     </row>
     <row r="19" spans="3:21">
       <c r="C19" s="15" t="s">
@@ -1540,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="19">
-        <f t="shared" ref="F21:M30" si="5">(((POWER($C22,F$19))-(POWER($C22,2)))/($C22-1))+(2*$C22)</f>
+        <f t="shared" ref="F22:M30" si="5">(((POWER($C22,F$19))-(POWER($C22,2)))/($C22-1))+(2*$C22)</f>
         <v>8</v>
       </c>
       <c r="G22" s="19">
@@ -2024,7 +2025,7 @@
   <dimension ref="B2:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:S45"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -3000,8 +3001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52EDCC2-98A0-234B-B823-E37B4CA5F8D0}">
   <dimension ref="AH3:BY1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BA1" sqref="BA1:CJ20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -3526,59 +3527,59 @@
       <c r="AI22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AJ22" s="21" t="s">
+      <c r="AJ22" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AK22" s="21"/>
-      <c r="AL22" s="21" t="s">
+      <c r="AK22" s="23"/>
+      <c r="AL22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AM22" s="21"/>
-      <c r="AN22" s="21"/>
-      <c r="AO22" s="21"/>
-      <c r="AP22" s="21" t="s">
+      <c r="AM22" s="23"/>
+      <c r="AN22" s="23"/>
+      <c r="AO22" s="23"/>
+      <c r="AP22" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AQ22" s="21"/>
-      <c r="AR22" s="21"/>
-      <c r="AS22" s="21"/>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
-      <c r="AV22" s="21"/>
-      <c r="AW22" s="21"/>
+      <c r="AQ22" s="23"/>
+      <c r="AR22" s="23"/>
+      <c r="AS22" s="23"/>
+      <c r="AT22" s="23"/>
+      <c r="AU22" s="23"/>
+      <c r="AV22" s="23"/>
+      <c r="AW22" s="23"/>
       <c r="BB22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BC22" s="21" t="s">
+      <c r="BC22" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="BD22" s="21"/>
-      <c r="BE22" s="21" t="s">
+      <c r="BD22" s="23"/>
+      <c r="BE22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="BF22" s="21"/>
-      <c r="BG22" s="21"/>
-      <c r="BH22" s="21"/>
-      <c r="BI22" s="21" t="s">
+      <c r="BF22" s="23"/>
+      <c r="BG22" s="23"/>
+      <c r="BH22" s="23"/>
+      <c r="BI22" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="BJ22" s="21"/>
-      <c r="BK22" s="21"/>
-      <c r="BL22" s="21"/>
-      <c r="BM22" s="21"/>
-      <c r="BN22" s="21"/>
-      <c r="BO22" s="21"/>
-      <c r="BP22" s="21"/>
-      <c r="BS22" s="21" t="s">
+      <c r="BJ22" s="23"/>
+      <c r="BK22" s="23"/>
+      <c r="BL22" s="23"/>
+      <c r="BM22" s="23"/>
+      <c r="BN22" s="23"/>
+      <c r="BO22" s="23"/>
+      <c r="BP22" s="23"/>
+      <c r="BS22" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="BT22" s="21"/>
-      <c r="BU22" s="21"/>
-      <c r="BW22" s="21" t="s">
+      <c r="BT22" s="23"/>
+      <c r="BU22" s="23"/>
+      <c r="BW22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="BX22" s="21"/>
-      <c r="BY22" s="21"/>
+      <c r="BX22" s="23"/>
+      <c r="BY22" s="23"/>
     </row>
     <row r="23" spans="34:77">
       <c r="AH23" s="5"/>
@@ -5545,4 +5546,211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07473FD9-618B-4656-9437-00E45B55D507}">
+  <dimension ref="A1:A189"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AS24" sqref="AS24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="182" width="1.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="2" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="3" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="4" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="5" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="6" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="7" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="8" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="9" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="10" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="11" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="12" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="13" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="14" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="15" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="16" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="17" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="18" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="19" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="20" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="21" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="22" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="23" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="24" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="25" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="26" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="27" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="28" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="29" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="30" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="31" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="32" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="33" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="34" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="35" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="36" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="37" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="38" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="39" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="40" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="41" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="42" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="43" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="44" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="45" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="46" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="47" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="48" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="49" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="50" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="51" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="52" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="53" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="54" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="55" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="56" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="57" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="58" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="59" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="60" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="61" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="62" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="63" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="64" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="65" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="66" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="67" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="68" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="69" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="70" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="71" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="72" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="73" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="74" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="75" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="76" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="77" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="78" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="79" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="80" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="81" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="82" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="83" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="84" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="85" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="86" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="87" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="88" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="89" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="90" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="91" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="92" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="93" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="94" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="95" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="96" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="97" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="98" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="99" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="100" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="101" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="102" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="103" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="104" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="105" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="106" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="107" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="108" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="109" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="110" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="111" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="112" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="113" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="114" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="115" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="116" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="117" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="118" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="119" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="120" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="121" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="122" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="123" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="124" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="125" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="126" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="127" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="128" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="129" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="130" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="131" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="132" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="133" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="134" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="135" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="136" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="137" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="138" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="139" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="140" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="141" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="142" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="143" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="144" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="145" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="146" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="147" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="148" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="149" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="150" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="151" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="152" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="153" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="154" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="155" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="156" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="157" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="158" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="159" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="160" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="161" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="162" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="163" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="164" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="165" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="166" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="167" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="168" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="169" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="170" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="171" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="172" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="173" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="174" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="175" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="176" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="177" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="178" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="179" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="180" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="181" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="182" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="183" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="184" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="185" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="186" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="187" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="188" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+    <row r="189" s="5" customFormat="1" ht="4.95" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementación del SIM-DJ realziada
</commit_message>
<xml_diff>
--- a/Jupyter Notebook/Cálculos de Matriz.xlsx
+++ b/Jupyter Notebook/Cálculos de Matriz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulise\Documents\UV\9° semestre\GTS\Jupyter Notebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulise\Documents\UV\9 semestre\GTS\Jupyter Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A4F04A-ADD0-4846-B234-F11AADBF23F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A290B4A-8522-4575-9A26-A54FC28D37D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2AA86D61-9D76-B74F-AA0D-E6B0A4E37F32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AA86D61-9D76-B74F-AA0D-E6B0A4E37F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Total de Escenarios Estrategias" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="100">
   <si>
     <t>a1</t>
   </si>
@@ -276,6 +276,72 @@
   </si>
   <si>
     <t>Cálculo de Decisiones totales A en el árbol</t>
+  </si>
+  <si>
+    <t>a1a3</t>
+  </si>
+  <si>
+    <t>a1a4</t>
+  </si>
+  <si>
+    <t>a2a3</t>
+  </si>
+  <si>
+    <t>a2a4</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>Z4</t>
+  </si>
+  <si>
+    <t>Resultado
+(zi)</t>
+  </si>
+  <si>
+    <t>Historia
+(hi)</t>
+  </si>
+  <si>
+    <t>Probabilidad
+Zi</t>
+  </si>
+  <si>
+    <t>Utilidad esperada</t>
+  </si>
+  <si>
+    <t>Piedra</t>
+  </si>
+  <si>
+    <t>Papel</t>
+  </si>
+  <si>
+    <t>Tijera</t>
+  </si>
+  <si>
+    <t>Jugador A</t>
+  </si>
+  <si>
+    <t>Jugador B</t>
+  </si>
+  <si>
+    <t>(0,0)</t>
+  </si>
+  <si>
+    <t>(+1,-1)</t>
+  </si>
+  <si>
+    <t>(-1,+1)</t>
+  </si>
+  <si>
+    <t>Cálculo de Historias totales h en el árbol</t>
   </si>
 </sst>
 </file>
@@ -285,7 +351,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,8 +390,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +444,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,10 +504,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -457,7 +537,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,9 +551,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,7 +594,7 @@
       <xdr:col>32</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>123705</xdr:rowOff>
+      <xdr:rowOff>32265</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -905,28 +1002,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C68D51D-B8CB-4062-B34D-A024901C524E}">
-  <dimension ref="B1:U37"/>
+  <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:O7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="2:19">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="2:19">
       <c r="B2" s="5"/>
@@ -1103,9 +1200,6 @@
         <f t="shared" si="4"/>
         <v>29524</v>
       </c>
-      <c r="O6">
-        <v>15</v>
-      </c>
       <c r="Q6">
         <v>40</v>
       </c>
@@ -1429,19 +1523,19 @@
       </c>
     </row>
     <row r="18" spans="3:21">
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="3:21">
       <c r="C19" s="15" t="s">
@@ -1934,87 +2028,530 @@
       </c>
     </row>
     <row r="32" spans="3:21">
-      <c r="D32" s="20">
-        <v>3</v>
-      </c>
-      <c r="F32" s="20">
-        <v>6</v>
-      </c>
-      <c r="H32">
-        <v>15</v>
-      </c>
-      <c r="J32">
-        <v>42</v>
-      </c>
-      <c r="L32">
-        <v>123</v>
-      </c>
-      <c r="N32">
-        <v>366</v>
-      </c>
       <c r="U32">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="5:13">
-      <c r="E33" s="20">
+    <row r="35" spans="3:13">
+      <c r="C35" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+    </row>
+    <row r="36" spans="3:13">
+      <c r="C36" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
+      <c r="E36" s="16">
+        <v>2</v>
+      </c>
+      <c r="F36" s="16">
         <v>3</v>
       </c>
-      <c r="G33" s="20">
+      <c r="G36" s="16">
+        <v>4</v>
+      </c>
+      <c r="H36" s="16">
+        <v>5</v>
+      </c>
+      <c r="I36" s="16">
+        <v>6</v>
+      </c>
+      <c r="J36" s="16">
+        <v>7</v>
+      </c>
+      <c r="K36" s="16">
+        <v>8</v>
+      </c>
+      <c r="L36" s="16">
         <v>9</v>
       </c>
-      <c r="I33">
+      <c r="M36" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13">
+      <c r="C37" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+    </row>
+    <row r="38" spans="3:13">
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18">
+        <f>POWER($C38,D$36)</f>
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
+        <f t="shared" ref="E38:M47" si="7">POWER($C38,E$36)</f>
+        <v>1</v>
+      </c>
+      <c r="F38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M38" s="18">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13">
+      <c r="C39" s="17">
+        <v>2</v>
+      </c>
+      <c r="D39" s="19">
+        <f>POWER($C39,D$36)</f>
+        <v>2</v>
+      </c>
+      <c r="E39" s="19">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F39" s="19">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G39" s="19">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="H39" s="19">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="I39" s="19">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+      <c r="K39" s="19">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+      <c r="L39" s="19">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13">
+      <c r="C40" s="17">
+        <v>3</v>
+      </c>
+      <c r="D40" s="19">
+        <f t="shared" ref="D40:D47" si="8">POWER($C40,D$36)</f>
+        <v>3</v>
+      </c>
+      <c r="E40" s="19">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="F40" s="19">
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="K33">
+      <c r="G40" s="19">
+        <f t="shared" si="7"/>
         <v>81</v>
       </c>
-      <c r="M33">
+      <c r="H40" s="19">
+        <f t="shared" si="7"/>
         <v>243</v>
       </c>
-    </row>
-    <row r="34" spans="5:13">
-      <c r="F34" s="20">
+      <c r="I40" s="19">
+        <f t="shared" si="7"/>
+        <v>729</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="7"/>
+        <v>2187</v>
+      </c>
+      <c r="K40" s="19">
+        <f t="shared" si="7"/>
+        <v>6561</v>
+      </c>
+      <c r="L40" s="19">
+        <f t="shared" si="7"/>
+        <v>19683</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="7"/>
+        <v>59049</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13">
+      <c r="C41" s="17">
+        <v>4</v>
+      </c>
+      <c r="D41" s="19">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E41" s="19">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="F41" s="19">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="G41" s="19">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+      <c r="H41" s="19">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+      <c r="I41" s="19">
+        <f t="shared" si="7"/>
+        <v>4096</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+      <c r="K41" s="19">
+        <f t="shared" si="7"/>
+        <v>65536</v>
+      </c>
+      <c r="L41" s="19">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="M41" s="19">
+        <f t="shared" si="7"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13">
+      <c r="C42" s="17">
+        <v>5</v>
+      </c>
+      <c r="D42" s="19">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E42" s="19">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="F42" s="19">
+        <f t="shared" si="7"/>
+        <v>125</v>
+      </c>
+      <c r="G42" s="19">
+        <f t="shared" si="7"/>
+        <v>625</v>
+      </c>
+      <c r="H42" s="19">
+        <f t="shared" si="7"/>
+        <v>3125</v>
+      </c>
+      <c r="I42" s="19">
+        <f t="shared" si="7"/>
+        <v>15625</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" si="7"/>
+        <v>78125</v>
+      </c>
+      <c r="K42" s="19">
+        <f t="shared" si="7"/>
+        <v>390625</v>
+      </c>
+      <c r="L42" s="19">
+        <f t="shared" si="7"/>
+        <v>1953125</v>
+      </c>
+      <c r="M42" s="19">
+        <f t="shared" si="7"/>
+        <v>9765625</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13">
+      <c r="C43" s="17">
         <v>6</v>
       </c>
-      <c r="H34">
-        <v>18</v>
-      </c>
-      <c r="J34">
-        <v>54</v>
-      </c>
-      <c r="L34">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="5:13">
-      <c r="G35">
-        <v>12</v>
-      </c>
-      <c r="I35">
+      <c r="D43" s="19">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E43" s="19">
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="K35">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="5:13">
-      <c r="H36">
-        <v>24</v>
-      </c>
-      <c r="J36">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="5:13">
-      <c r="I37">
-        <v>48</v>
+      <c r="F43" s="19">
+        <f t="shared" si="7"/>
+        <v>216</v>
+      </c>
+      <c r="G43" s="19">
+        <f t="shared" si="7"/>
+        <v>1296</v>
+      </c>
+      <c r="H43" s="19">
+        <f t="shared" si="7"/>
+        <v>7776</v>
+      </c>
+      <c r="I43" s="19">
+        <f t="shared" si="7"/>
+        <v>46656</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="7"/>
+        <v>279936</v>
+      </c>
+      <c r="K43" s="19">
+        <f t="shared" si="7"/>
+        <v>1679616</v>
+      </c>
+      <c r="L43" s="19">
+        <f t="shared" si="7"/>
+        <v>10077696</v>
+      </c>
+      <c r="M43" s="19">
+        <f t="shared" si="7"/>
+        <v>60466176</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13">
+      <c r="C44" s="17">
+        <v>7</v>
+      </c>
+      <c r="D44" s="19">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E44" s="19">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="F44" s="19">
+        <f t="shared" si="7"/>
+        <v>343</v>
+      </c>
+      <c r="G44" s="19">
+        <f t="shared" si="7"/>
+        <v>2401</v>
+      </c>
+      <c r="H44" s="19">
+        <f t="shared" si="7"/>
+        <v>16807</v>
+      </c>
+      <c r="I44" s="19">
+        <f t="shared" si="7"/>
+        <v>117649</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="7"/>
+        <v>823543</v>
+      </c>
+      <c r="K44" s="19">
+        <f t="shared" si="7"/>
+        <v>5764801</v>
+      </c>
+      <c r="L44" s="19">
+        <f t="shared" si="7"/>
+        <v>40353607</v>
+      </c>
+      <c r="M44" s="19">
+        <f t="shared" si="7"/>
+        <v>282475249</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13">
+      <c r="C45" s="17">
+        <v>8</v>
+      </c>
+      <c r="D45" s="19">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="E45" s="19">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="F45" s="19">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+      <c r="G45" s="19">
+        <f t="shared" si="7"/>
+        <v>4096</v>
+      </c>
+      <c r="H45" s="19">
+        <f t="shared" si="7"/>
+        <v>32768</v>
+      </c>
+      <c r="I45" s="19">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" si="7"/>
+        <v>2097152</v>
+      </c>
+      <c r="K45" s="19">
+        <f t="shared" si="7"/>
+        <v>16777216</v>
+      </c>
+      <c r="L45" s="19">
+        <f t="shared" si="7"/>
+        <v>134217728</v>
+      </c>
+      <c r="M45" s="19">
+        <f t="shared" si="7"/>
+        <v>1073741824</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13">
+      <c r="C46" s="17">
+        <v>9</v>
+      </c>
+      <c r="D46" s="19">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="E46" s="19">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>729</v>
+      </c>
+      <c r="G46" s="19">
+        <f t="shared" si="7"/>
+        <v>6561</v>
+      </c>
+      <c r="H46" s="19">
+        <f t="shared" si="7"/>
+        <v>59049</v>
+      </c>
+      <c r="I46" s="19">
+        <f t="shared" si="7"/>
+        <v>531441</v>
+      </c>
+      <c r="J46" s="19">
+        <f t="shared" si="7"/>
+        <v>4782969</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="7"/>
+        <v>43046721</v>
+      </c>
+      <c r="L46" s="19">
+        <f t="shared" si="7"/>
+        <v>387420489</v>
+      </c>
+      <c r="M46" s="19">
+        <f t="shared" si="7"/>
+        <v>3486784401</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13">
+      <c r="C47" s="17">
+        <v>10</v>
+      </c>
+      <c r="D47" s="19">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="E47" s="19">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="F47" s="19">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="G47" s="19">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="H47" s="19">
+        <f t="shared" si="7"/>
+        <v>100000</v>
+      </c>
+      <c r="I47" s="19">
+        <f t="shared" si="7"/>
+        <v>1000000</v>
+      </c>
+      <c r="J47" s="19">
+        <f t="shared" si="7"/>
+        <v>10000000</v>
+      </c>
+      <c r="K47" s="19">
+        <f t="shared" si="7"/>
+        <v>100000000</v>
+      </c>
+      <c r="L47" s="19">
+        <f t="shared" si="7"/>
+        <v>1000000000</v>
+      </c>
+      <c r="M47" s="19">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:M1"/>
     <mergeCell ref="C18:M18"/>
+    <mergeCell ref="C35:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2999,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52EDCC2-98A0-234B-B823-E37B4CA5F8D0}">
-  <dimension ref="AH3:BY1048576"/>
+  <dimension ref="AH2:CF1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CC11" sqref="CC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -3022,18 +3559,42 @@
     <col min="53" max="53" width="10.5" bestFit="1" customWidth="1"/>
     <col min="54" max="58" width="5.296875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="9.19921875" customWidth="1"/>
-    <col min="60" max="66" width="5.296875" bestFit="1" customWidth="1"/>
+    <col min="60" max="63" width="5.296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="5.5" customWidth="1"/>
+    <col min="66" max="66" width="4.796875" customWidth="1"/>
     <col min="67" max="67" width="4.796875" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="5.296875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.59765625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="4.69921875" bestFit="1" customWidth="1"/>
     <col min="71" max="72" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="2.796875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="2" customWidth="1"/>
     <col min="75" max="77" width="8" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.19921875" customWidth="1"/>
+    <col min="80" max="80" width="3.19921875" customWidth="1"/>
+    <col min="81" max="81" width="6.19921875" customWidth="1"/>
+    <col min="82" max="84" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="34:49">
+    <row r="2" spans="34:84">
+      <c r="BH2" s="27"/>
+      <c r="BI2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK2" s="25"/>
+      <c r="BL2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="BM2" s="25"/>
+      <c r="BN2" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO2" s="25"/>
+    </row>
+    <row r="3" spans="34:84">
       <c r="AH3" s="5"/>
       <c r="AI3" s="5" t="s">
         <v>30</v>
@@ -3080,8 +3641,39 @@
       <c r="AW3" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="34:49">
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BE3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH3" s="27"/>
+      <c r="BI3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BL3" s="25"/>
+      <c r="BM3" s="25"/>
+      <c r="BN3" s="25"/>
+      <c r="BO3" s="25"/>
+      <c r="CB3" s="27"/>
+      <c r="CC3" s="27"/>
+      <c r="CD3" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="CE3" s="25"/>
+      <c r="CF3" s="25"/>
+    </row>
+    <row r="4" spans="34:84">
       <c r="AH4" s="5" t="s">
         <v>0</v>
       </c>
@@ -3102,8 +3694,45 @@
       <c r="AU4" s="5"/>
       <c r="AV4" s="5"/>
       <c r="AW4" s="5"/>
-    </row>
-    <row r="5" spans="34:49">
+      <c r="BC4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BE4" s="5"/>
+      <c r="BF4" s="5"/>
+      <c r="BH4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BI4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK4" s="5"/>
+      <c r="BL4" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM4" s="25"/>
+      <c r="BN4" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO4" s="25"/>
+      <c r="CB4" s="27"/>
+      <c r="CC4" s="27"/>
+      <c r="CD4" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="CE4" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF4" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="34:84" ht="18" customHeight="1">
       <c r="AH5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3124,8 +3753,49 @@
       <c r="AU5" s="5"/>
       <c r="AV5" s="5"/>
       <c r="AW5" s="5"/>
-    </row>
-    <row r="6" spans="34:49">
+      <c r="BC5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BE5" s="5"/>
+      <c r="BF5" s="5"/>
+      <c r="BH5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="BI5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK5" s="5"/>
+      <c r="BL5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM5" s="25"/>
+      <c r="BN5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO5" s="25"/>
+      <c r="CB5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="CC5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="CD5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="CE5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="CF5" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="34:84" ht="18" customHeight="1">
       <c r="AH6" s="5" t="s">
         <v>2</v>
       </c>
@@ -3148,8 +3818,49 @@
       <c r="AU6" s="5"/>
       <c r="AV6" s="5"/>
       <c r="AW6" s="5"/>
-    </row>
-    <row r="7" spans="34:49">
+      <c r="BC6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD6" s="5"/>
+      <c r="BE6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BF6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BH6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BJ6" s="5"/>
+      <c r="BK6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL6" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="BM6" s="25"/>
+      <c r="BN6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO6" s="25"/>
+      <c r="CB6" s="26"/>
+      <c r="CC6" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="CD6" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="CE6" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="CF6" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="34:84" ht="18" customHeight="1">
       <c r="AH7" s="5" t="s">
         <v>3</v>
       </c>
@@ -3172,8 +3883,49 @@
       <c r="AU7" s="5"/>
       <c r="AV7" s="5"/>
       <c r="AW7" s="5"/>
-    </row>
-    <row r="8" spans="34:49">
+      <c r="BC7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD7" s="5"/>
+      <c r="BE7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BF7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BH7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BJ7" s="5"/>
+      <c r="BK7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="BM7" s="25"/>
+      <c r="BN7" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="BO7" s="25"/>
+      <c r="CB7" s="26"/>
+      <c r="CC7" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="CD7" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="CE7" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="CF7" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="34:84">
       <c r="AH8" s="5" t="s">
         <v>4</v>
       </c>
@@ -3194,8 +3946,14 @@
       <c r="AU8" s="5"/>
       <c r="AV8" s="5"/>
       <c r="AW8" s="5"/>
-    </row>
-    <row r="9" spans="34:49">
+      <c r="BS8" t="s">
+        <v>47</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="34:84">
       <c r="AH9" s="5" t="s">
         <v>5</v>
       </c>
@@ -3216,8 +3974,24 @@
       <c r="AU9" s="5"/>
       <c r="AV9" s="5"/>
       <c r="AW9" s="5"/>
-    </row>
-    <row r="10" spans="34:49">
+      <c r="BH9" s="27"/>
+      <c r="BI9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK9" s="25"/>
+      <c r="BL9" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM9" s="25"/>
+      <c r="BW9" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="BX9" s="25"/>
+    </row>
+    <row r="10" spans="34:84">
       <c r="AH10" s="5" t="s">
         <v>6</v>
       </c>
@@ -3238,8 +4012,32 @@
       <c r="AU10" s="5"/>
       <c r="AV10" s="5"/>
       <c r="AW10" s="5"/>
-    </row>
-    <row r="11" spans="34:49">
+      <c r="BH10" s="27"/>
+      <c r="BI10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BL10" s="25"/>
+      <c r="BM10" s="25"/>
+      <c r="BS10" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="BT10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="BW10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="BX10" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="34:84">
       <c r="AH11" s="5" t="s">
         <v>7</v>
       </c>
@@ -3260,8 +4058,38 @@
       <c r="AU11" s="5"/>
       <c r="AV11" s="5"/>
       <c r="AW11" s="5"/>
-    </row>
-    <row r="12" spans="34:49">
+      <c r="BH11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BI11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BJ11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BK11" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL11" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="BM11" s="25"/>
+      <c r="BS11" s="22">
+        <v>1</v>
+      </c>
+      <c r="BT11" s="22">
+        <v>1</v>
+      </c>
+      <c r="BW11" s="5">
+        <f>BL11*BS11</f>
+        <v>0.25</v>
+      </c>
+      <c r="BX11" s="5">
+        <f>BL11*BT11</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="34:84">
       <c r="AH12" s="5" t="s">
         <v>8</v>
       </c>
@@ -3282,8 +4110,38 @@
       <c r="AU12" s="5"/>
       <c r="AV12" s="5"/>
       <c r="AW12" s="5"/>
-    </row>
-    <row r="13" spans="34:49">
+      <c r="BH12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="BI12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BJ12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BK12" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL12" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="BM12" s="25"/>
+      <c r="BS12" s="22">
+        <v>0</v>
+      </c>
+      <c r="BT12" s="22">
+        <v>0</v>
+      </c>
+      <c r="BW12" s="5">
+        <f t="shared" ref="BW12:BW14" si="0">BL12*BS12</f>
+        <v>0</v>
+      </c>
+      <c r="BX12" s="5">
+        <f t="shared" ref="BX12:BX14" si="1">BL12*BT12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="34:84">
       <c r="AH13" s="5" t="s">
         <v>9</v>
       </c>
@@ -3304,8 +4162,38 @@
       <c r="AU13" s="5"/>
       <c r="AV13" s="5"/>
       <c r="AW13" s="5"/>
-    </row>
-    <row r="14" spans="34:49">
+      <c r="BH13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BJ13" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BL13" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="BM13" s="25"/>
+      <c r="BS13" s="22">
+        <v>0</v>
+      </c>
+      <c r="BT13" s="22">
+        <v>0</v>
+      </c>
+      <c r="BW13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="BX13" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="34:84">
       <c r="AH14" s="5" t="s">
         <v>10</v>
       </c>
@@ -3326,8 +4214,38 @@
       <c r="AU14" s="5"/>
       <c r="AV14" s="5"/>
       <c r="AW14" s="5"/>
-    </row>
-    <row r="15" spans="34:49">
+      <c r="BH14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BJ14" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="BL14" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="BM14" s="25"/>
+      <c r="BS14" s="22">
+        <v>1</v>
+      </c>
+      <c r="BT14" s="22">
+        <v>1</v>
+      </c>
+      <c r="BW14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="BX14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="34:84">
       <c r="AH15" s="5" t="s">
         <v>11</v>
       </c>
@@ -3349,7 +4267,7 @@
       <c r="AV15" s="5"/>
       <c r="AW15" s="5"/>
     </row>
-    <row r="16" spans="34:49">
+    <row r="16" spans="34:84">
       <c r="AH16" s="5" t="s">
         <v>12</v>
       </c>
@@ -3467,59 +4385,59 @@
         <v>1</v>
       </c>
       <c r="AJ20">
-        <f t="shared" ref="AJ20:AW20" si="0">SUM(AJ4:AJ19)</f>
+        <f t="shared" ref="AJ20:AW20" si="2">SUM(AJ4:AJ19)</f>
         <v>1</v>
       </c>
       <c r="AK20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AM20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AN20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AO20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AQ20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AR20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AS20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AT20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AU20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AV20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AW20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3527,59 +4445,59 @@
       <c r="AI22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AJ22" s="23" t="s">
+      <c r="AJ22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="AK22" s="23"/>
-      <c r="AL22" s="23" t="s">
+      <c r="AK22" s="25"/>
+      <c r="AL22" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="AM22" s="23"/>
-      <c r="AN22" s="23"/>
-      <c r="AO22" s="23"/>
-      <c r="AP22" s="23" t="s">
+      <c r="AM22" s="25"/>
+      <c r="AN22" s="25"/>
+      <c r="AO22" s="25"/>
+      <c r="AP22" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="AQ22" s="23"/>
-      <c r="AR22" s="23"/>
-      <c r="AS22" s="23"/>
-      <c r="AT22" s="23"/>
-      <c r="AU22" s="23"/>
-      <c r="AV22" s="23"/>
-      <c r="AW22" s="23"/>
+      <c r="AQ22" s="25"/>
+      <c r="AR22" s="25"/>
+      <c r="AS22" s="25"/>
+      <c r="AT22" s="25"/>
+      <c r="AU22" s="25"/>
+      <c r="AV22" s="25"/>
+      <c r="AW22" s="25"/>
       <c r="BB22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BC22" s="23" t="s">
+      <c r="BC22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="BD22" s="23"/>
-      <c r="BE22" s="23" t="s">
+      <c r="BD22" s="25"/>
+      <c r="BE22" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="BF22" s="23"/>
-      <c r="BG22" s="23"/>
-      <c r="BH22" s="23"/>
-      <c r="BI22" s="23" t="s">
+      <c r="BF22" s="25"/>
+      <c r="BG22" s="25"/>
+      <c r="BH22" s="25"/>
+      <c r="BI22" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="BJ22" s="23"/>
-      <c r="BK22" s="23"/>
-      <c r="BL22" s="23"/>
-      <c r="BM22" s="23"/>
-      <c r="BN22" s="23"/>
-      <c r="BO22" s="23"/>
-      <c r="BP22" s="23"/>
-      <c r="BS22" s="23" t="s">
+      <c r="BJ22" s="25"/>
+      <c r="BK22" s="25"/>
+      <c r="BL22" s="25"/>
+      <c r="BM22" s="25"/>
+      <c r="BN22" s="25"/>
+      <c r="BO22" s="25"/>
+      <c r="BP22" s="25"/>
+      <c r="BS22" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="BT22" s="23"/>
-      <c r="BU22" s="23"/>
-      <c r="BW22" s="23" t="s">
+      <c r="BT22" s="25"/>
+      <c r="BU22" s="25"/>
+      <c r="BW22" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="BX22" s="23"/>
-      <c r="BY22" s="23"/>
+      <c r="BX22" s="25"/>
+      <c r="BY22" s="25"/>
     </row>
     <row r="23" spans="34:77">
       <c r="AH23" s="5"/>
@@ -3786,7 +4704,7 @@
       <c r="BP24" s="7">
         <v>1</v>
       </c>
-      <c r="BQ24" s="6">
+      <c r="BQ24" s="21">
         <f>BB24*BC24*BD24*BE24*BF24*BG24*BH24*BI24*BJ24*BK24*BL24*BM24*BN24*BO24*BP24</f>
         <v>6.1199999999999991E-2</v>
       </c>
@@ -3843,7 +4761,7 @@
       <c r="AV25" s="7"/>
       <c r="AW25" s="7"/>
       <c r="AX25" s="11" t="str">
-        <f t="shared" ref="AX25:AX39" si="1">_xlfn.TEXTJOIN("", 0,AI25:AW25)</f>
+        <f t="shared" ref="AX25:AX39" si="3">_xlfn.TEXTJOIN("", 0,AI25:AW25)</f>
         <v>a1a3a5a14</v>
       </c>
       <c r="AY25" s="9" t="s">
@@ -3853,7 +4771,7 @@
         <v>32</v>
       </c>
       <c r="BB25" s="8">
-        <f t="shared" ref="BB25:BB31" si="2">$AI$4</f>
+        <f t="shared" ref="BB25:BB31" si="4">$AI$4</f>
         <v>0.4</v>
       </c>
       <c r="BC25" s="8">
@@ -3898,8 +4816,8 @@
       <c r="BP25" s="7">
         <v>1</v>
       </c>
-      <c r="BQ25" s="6">
-        <f t="shared" ref="BQ25:BQ39" si="3">BB25*BC25*BD25*BE25*BF25*BG25*BH25*BI25*BJ25*BK25*BL25*BM25*BN25*BO25*BP25</f>
+      <c r="BQ25" s="21">
+        <f t="shared" ref="BQ25:BQ39" si="5">BB25*BC25*BD25*BE25*BF25*BG25*BH25*BI25*BJ25*BK25*BL25*BM25*BN25*BO25*BP25</f>
         <v>4.0800000000000003E-2</v>
       </c>
       <c r="BR25" t="s">
@@ -3915,15 +4833,15 @@
         <v>2</v>
       </c>
       <c r="BW25" s="5">
-        <f t="shared" ref="BW25:BW38" si="4">$BQ$24*BS25</f>
+        <f t="shared" ref="BW25:BW38" si="6">$BQ$24*BS25</f>
         <v>0.12239999999999998</v>
       </c>
       <c r="BX25" s="5">
-        <f t="shared" ref="BX25:BX39" si="5">$BQ$24*BT25</f>
+        <f t="shared" ref="BX25:BX39" si="7">$BQ$24*BT25</f>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY25" s="5">
-        <f t="shared" ref="BY25:BY39" si="6">$BQ$24*BU25</f>
+        <f t="shared" ref="BY25:BY39" si="8">$BQ$24*BU25</f>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -3955,7 +4873,7 @@
       <c r="AV26" s="7"/>
       <c r="AW26" s="7"/>
       <c r="AX26" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a3a6a13</v>
       </c>
       <c r="AY26" s="9" t="s">
@@ -3965,7 +4883,7 @@
         <v>33</v>
       </c>
       <c r="BB26" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC26" s="8">
@@ -4011,8 +4929,8 @@
       <c r="BP26" s="7">
         <v>1</v>
       </c>
-      <c r="BQ26" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ26" s="21">
+        <f t="shared" si="5"/>
         <v>1.44E-2</v>
       </c>
       <c r="BR26" t="s">
@@ -4028,15 +4946,15 @@
         <v>3</v>
       </c>
       <c r="BW26" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX26" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.12239999999999998</v>
       </c>
       <c r="BY26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.18359999999999999</v>
       </c>
     </row>
@@ -4068,7 +4986,7 @@
       <c r="AV27" s="7"/>
       <c r="AW27" s="7"/>
       <c r="AX27" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a3a6a14</v>
       </c>
       <c r="AY27" s="9" t="s">
@@ -4078,7 +4996,7 @@
         <v>34</v>
       </c>
       <c r="BB27" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC27" s="8">
@@ -4123,8 +5041,8 @@
       <c r="BP27" s="7">
         <v>1</v>
       </c>
-      <c r="BQ27" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ27" s="21">
+        <f t="shared" si="5"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="BR27" t="s">
@@ -4140,15 +5058,15 @@
         <v>2</v>
       </c>
       <c r="BW27" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BX27" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -4180,7 +5098,7 @@
       <c r="AV28" s="7"/>
       <c r="AW28" s="7"/>
       <c r="AX28" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a4a7a13</v>
       </c>
       <c r="AY28" s="9" t="s">
@@ -4190,7 +5108,7 @@
         <v>35</v>
       </c>
       <c r="BB28" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC28" s="8">
@@ -4235,8 +5153,8 @@
       <c r="BP28" s="7">
         <v>1</v>
       </c>
-      <c r="BQ28" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ28" s="21">
+        <f t="shared" si="5"/>
         <v>2.6459999999999994E-2</v>
       </c>
       <c r="BR28" t="s">
@@ -4252,15 +5170,15 @@
         <v>3</v>
       </c>
       <c r="BW28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.12239999999999998</v>
       </c>
       <c r="BX28" s="5">
-        <f t="shared" ref="BX28:BX35" si="7">$BQ$24*BT28</f>
+        <f t="shared" ref="BX28:BX35" si="9">$BQ$24*BT28</f>
         <v>0.24479999999999996</v>
       </c>
       <c r="BY28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.18359999999999999</v>
       </c>
     </row>
@@ -4292,7 +5210,7 @@
       <c r="AV29" s="7"/>
       <c r="AW29" s="7"/>
       <c r="AX29" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a4a7a14</v>
       </c>
       <c r="AY29" s="9" t="s">
@@ -4302,7 +5220,7 @@
         <v>36</v>
       </c>
       <c r="BB29" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC29" s="8">
@@ -4347,8 +5265,8 @@
       <c r="BP29" s="7">
         <v>1</v>
       </c>
-      <c r="BQ29" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ29" s="21">
+        <f t="shared" si="5"/>
         <v>0.14993999999999996</v>
       </c>
       <c r="BR29" t="s">
@@ -4364,15 +5282,15 @@
         <v>2</v>
       </c>
       <c r="BW29" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -4404,7 +5322,7 @@
       <c r="AV30" s="7"/>
       <c r="AW30" s="7"/>
       <c r="AX30" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a4a8a13</v>
       </c>
       <c r="AY30" s="9" t="s">
@@ -4414,7 +5332,7 @@
         <v>37</v>
       </c>
       <c r="BB30" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC30" s="8">
@@ -4459,8 +5377,8 @@
       <c r="BP30" s="7">
         <v>1</v>
       </c>
-      <c r="BQ30" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ30" s="21">
+        <f t="shared" si="5"/>
         <v>2.3827999999999998E-2</v>
       </c>
       <c r="BR30" t="s">
@@ -4476,15 +5394,15 @@
         <v>3</v>
       </c>
       <c r="BW30" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="BX30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BY30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.18359999999999999</v>
       </c>
     </row>
@@ -4516,7 +5434,7 @@
       <c r="AV31" s="6"/>
       <c r="AW31" s="7"/>
       <c r="AX31" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a1a4a8a14</v>
       </c>
       <c r="AY31" s="9" t="s">
@@ -4526,7 +5444,7 @@
         <v>38</v>
       </c>
       <c r="BB31" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="BC31" s="8">
@@ -4571,8 +5489,8 @@
       <c r="BP31" s="7">
         <v>1</v>
       </c>
-      <c r="BQ31" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ31" s="21">
+        <f t="shared" si="5"/>
         <v>7.9771999999999996E-2</v>
       </c>
       <c r="BR31" t="s">
@@ -4588,15 +5506,15 @@
         <v>2</v>
       </c>
       <c r="BW31" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BX31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -4628,7 +5546,7 @@
       <c r="AV32" s="6"/>
       <c r="AW32" s="7"/>
       <c r="AX32" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a3a9a15</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -4683,8 +5601,8 @@
       <c r="BP32" s="7">
         <v>1</v>
       </c>
-      <c r="BQ32" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ32" s="21">
+        <f t="shared" si="5"/>
         <v>3.9689999999999996E-2</v>
       </c>
       <c r="BR32" t="s">
@@ -4700,15 +5618,15 @@
         <v>-1</v>
       </c>
       <c r="BW32" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX32" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BY32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-6.1199999999999991E-2</v>
       </c>
     </row>
@@ -4740,7 +5658,7 @@
       <c r="AV33" s="6"/>
       <c r="AW33" s="7"/>
       <c r="AX33" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a3a9a16</v>
       </c>
       <c r="AY33" s="9" t="s">
@@ -4750,7 +5668,7 @@
         <v>40</v>
       </c>
       <c r="BB33" s="8">
-        <f t="shared" ref="BB33:BB39" si="8">$AI$5</f>
+        <f t="shared" ref="BB33:BB39" si="10">$AI$5</f>
         <v>0.6</v>
       </c>
       <c r="BC33" s="7">
@@ -4795,8 +5713,8 @@
       <c r="BP33" s="7">
         <v>1</v>
       </c>
-      <c r="BQ33" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ33" s="21">
+        <f t="shared" si="5"/>
         <v>7.3709999999999998E-2</v>
       </c>
       <c r="BR33" t="s">
@@ -4812,15 +5730,15 @@
         <v>2</v>
       </c>
       <c r="BW33" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BX33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -4852,7 +5770,7 @@
       <c r="AV34" s="6"/>
       <c r="AW34" s="7"/>
       <c r="AX34" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a3a10a15</v>
       </c>
       <c r="AY34" s="9" t="s">
@@ -4862,7 +5780,7 @@
         <v>41</v>
       </c>
       <c r="BB34" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC34" s="7">
@@ -4907,8 +5825,8 @@
       <c r="BP34" s="7">
         <v>1</v>
       </c>
-      <c r="BQ34" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ34" s="21">
+        <f t="shared" si="5"/>
         <v>0.27594000000000002</v>
       </c>
       <c r="BR34" t="s">
@@ -4924,15 +5842,15 @@
         <v>-1</v>
       </c>
       <c r="BW34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.12239999999999998</v>
       </c>
       <c r="BX34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-6.1199999999999991E-2</v>
       </c>
       <c r="BY34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-6.1199999999999991E-2</v>
       </c>
     </row>
@@ -4964,7 +5882,7 @@
       <c r="AV35" s="6"/>
       <c r="AW35" s="7"/>
       <c r="AX35" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a3a10a16</v>
       </c>
       <c r="AY35" s="9" t="s">
@@ -4974,7 +5892,7 @@
         <v>42</v>
       </c>
       <c r="BB35" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC35" s="7">
@@ -5019,8 +5937,8 @@
       <c r="BP35" s="7">
         <v>1</v>
       </c>
-      <c r="BQ35" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ35" s="21">
+        <f t="shared" si="5"/>
         <v>3.066E-2</v>
       </c>
       <c r="BR35" t="s">
@@ -5036,15 +5954,15 @@
         <v>2</v>
       </c>
       <c r="BW35" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX35" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BY35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -5075,7 +5993,7 @@
         <v>14</v>
       </c>
       <c r="AX36" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a4a11a15</v>
       </c>
       <c r="AY36" s="9" t="s">
@@ -5085,7 +6003,7 @@
         <v>43</v>
       </c>
       <c r="BB36" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC36" s="7">
@@ -5130,8 +6048,8 @@
       <c r="BP36" s="7">
         <v>1</v>
       </c>
-      <c r="BQ36" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ36" s="21">
+        <f t="shared" si="5"/>
         <v>4.6800000000000001E-3</v>
       </c>
       <c r="BR36" t="s">
@@ -5147,15 +6065,15 @@
         <v>-1</v>
       </c>
       <c r="BW36" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX36" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.12239999999999998</v>
       </c>
       <c r="BY36" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-6.1199999999999991E-2</v>
       </c>
     </row>
@@ -5186,7 +6104,7 @@
         <v>15</v>
       </c>
       <c r="AX37" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a4a11a16</v>
       </c>
       <c r="AY37" s="9" t="s">
@@ -5196,7 +6114,7 @@
         <v>44</v>
       </c>
       <c r="BB37" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC37" s="7">
@@ -5241,8 +6159,8 @@
       <c r="BP37" s="7">
         <v>1</v>
       </c>
-      <c r="BQ37" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ37" s="21">
+        <f t="shared" si="5"/>
         <v>1.8720000000000001E-2</v>
       </c>
       <c r="BR37" t="s">
@@ -5258,15 +6176,15 @@
         <v>2</v>
       </c>
       <c r="BW37" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.12239999999999998</v>
       </c>
       <c r="BX37" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BY37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -5298,7 +6216,7 @@
         <v>14</v>
       </c>
       <c r="AX38" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a4a12a15</v>
       </c>
       <c r="AY38" s="9" t="s">
@@ -5308,7 +6226,7 @@
         <v>45</v>
       </c>
       <c r="BB38" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC38" s="7">
@@ -5353,8 +6271,8 @@
       <c r="BP38" s="8">
         <v>0.3</v>
       </c>
-      <c r="BQ38" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ38" s="21">
+        <f t="shared" si="5"/>
         <v>4.6979999999999994E-2</v>
       </c>
       <c r="BR38" t="s">
@@ -5370,15 +6288,15 @@
         <v>-1</v>
       </c>
       <c r="BW38" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.24479999999999996</v>
       </c>
       <c r="BX38" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.12239999999999998</v>
       </c>
       <c r="BY38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-6.1199999999999991E-2</v>
       </c>
     </row>
@@ -5410,7 +6328,7 @@
         <v>15</v>
       </c>
       <c r="AX39" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>a2a4a12a16</v>
       </c>
       <c r="AY39" s="9" t="s">
@@ -5420,7 +6338,7 @@
         <v>46</v>
       </c>
       <c r="BB39" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="BC39" s="7">
@@ -5465,8 +6383,8 @@
       <c r="BP39" s="8">
         <v>0.7</v>
       </c>
-      <c r="BQ39" s="6">
-        <f t="shared" si="3"/>
+      <c r="BQ39" s="21">
+        <f t="shared" si="5"/>
         <v>0.10961999999999998</v>
       </c>
       <c r="BR39" t="s">
@@ -5486,11 +6404,11 @@
         <v>6.1199999999999991E-2</v>
       </c>
       <c r="BX39" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.18359999999999999</v>
       </c>
       <c r="BY39" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.12239999999999998</v>
       </c>
     </row>
@@ -5520,15 +6438,38 @@
       <c r="AY1048576" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AL22:AO22"/>
-    <mergeCell ref="AP22:AW22"/>
+  <mergeCells count="31">
     <mergeCell ref="BS22:BU22"/>
     <mergeCell ref="BW22:BY22"/>
     <mergeCell ref="BC22:BD22"/>
     <mergeCell ref="BE22:BH22"/>
     <mergeCell ref="BI22:BP22"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BL4:BM4"/>
+    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AL22:AO22"/>
+    <mergeCell ref="AP22:AW22"/>
+    <mergeCell ref="BL13:BM13"/>
+    <mergeCell ref="BL14:BM14"/>
+    <mergeCell ref="BH9:BH10"/>
+    <mergeCell ref="BJ9:BK9"/>
+    <mergeCell ref="BL9:BM10"/>
+    <mergeCell ref="BL11:BM11"/>
+    <mergeCell ref="BW9:BX9"/>
+    <mergeCell ref="CD3:CF3"/>
+    <mergeCell ref="CB5:CB7"/>
+    <mergeCell ref="CB3:CC4"/>
+    <mergeCell ref="BL12:BM12"/>
+    <mergeCell ref="BL6:BM6"/>
+    <mergeCell ref="BL7:BM7"/>
+    <mergeCell ref="BN4:BO4"/>
+    <mergeCell ref="BN5:BO5"/>
+    <mergeCell ref="BN6:BO6"/>
+    <mergeCell ref="BN7:BO7"/>
+    <mergeCell ref="BL2:BM3"/>
+    <mergeCell ref="BN2:BO3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="BW24:BY39">
@@ -5544,7 +6485,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>